<commit_message>
fix: stable version with search and safe stock handling
</commit_message>
<xml_diff>
--- a/data/catalog.xlsx
+++ b/data/catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\jmd_store_render\jmd_store\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C1FD8B-D7C9-4240-85D9-68A6C35AE084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AAB713-7A55-4BEB-BBA1-BF43A1DD9BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nike" sheetId="3" r:id="rId1"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50E1A44-280D-4411-9C01-14D3EB718FB5}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="K1:L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>28</v>
@@ -872,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC76538-67CE-4574-A08C-7F9575FC0AF6}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>